<commit_message>
among other things, pic comparing the coulomb log based on cary's formula and the one in nrl
</commit_message>
<xml_diff>
--- a/orfeas_competition/Mirror0D.xlsx
+++ b/orfeas_competition/Mirror0D.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/Python Scripts/orfeas_competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{C9E569C6-D225-2449-81CE-F63B9459901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66E8A7CB-4A44-47A2-A6DD-10609C7DEA7D}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{C9E569C6-D225-2449-81CE-F63B9459901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9C307E8-E450-41C3-813B-78CFD08C0D8B}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FD75F1BD-3419-8A42-869C-4E4296CA182A}"/>
   </bookViews>
@@ -79,7 +79,6 @@
     <definedName name="Zeff">Sheet1!$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -121,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="221">
   <si>
     <t>ngyro</t>
   </si>
@@ -775,6 +774,15 @@
   </si>
   <si>
     <t>keV</t>
+  </si>
+  <si>
+    <t>What is this?</t>
+  </si>
+  <si>
+    <t>How?</t>
+  </si>
+  <si>
+    <t>Source?</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6664DC-0609-414F-AD6B-0794283356C6}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="101" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="D187" sqref="D187"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="101" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.7"/>
@@ -1610,6 +1618,9 @@
       </c>
     </row>
     <row r="22" spans="1:19">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -2054,6 +2065,9 @@
       <c r="Q42" s="2"/>
     </row>
     <row r="43" spans="1:17">
+      <c r="A43" t="s">
+        <v>218</v>
+      </c>
       <c r="B43" t="s">
         <v>208</v>
       </c>
@@ -2143,7 +2157,7 @@
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
     </row>
-    <row r="49" spans="2:18">
+    <row r="49" spans="1:18">
       <c r="B49" t="s">
         <v>19</v>
       </c>
@@ -2166,7 +2180,7 @@
         <v>1.3010299956639813</v>
       </c>
     </row>
-    <row r="50" spans="2:18">
+    <row r="50" spans="1:18">
       <c r="B50" t="s">
         <v>20</v>
       </c>
@@ -2186,14 +2200,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="1:18">
       <c r="B51" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="2:18">
+    <row r="52" spans="1:18">
       <c r="B52" t="s">
         <v>18</v>
       </c>
@@ -2206,7 +2220,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="1:18">
       <c r="B53" t="s">
         <v>19</v>
       </c>
@@ -2215,7 +2229,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="1:18">
       <c r="B54" t="s">
         <v>20</v>
       </c>
@@ -2240,7 +2254,7 @@
         <v>32.940392293420615</v>
       </c>
     </row>
-    <row r="55" spans="2:18">
+    <row r="55" spans="1:18">
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="K55">
@@ -2253,7 +2267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:18">
+    <row r="56" spans="1:18">
       <c r="B56" t="s">
         <v>64</v>
       </c>
@@ -2274,14 +2288,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="2:18">
+    <row r="57" spans="1:18">
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="2:18">
+    <row r="58" spans="1:18">
       <c r="B58" t="s">
         <v>136</v>
       </c>
@@ -2302,14 +2316,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="2:18">
+    <row r="59" spans="1:18">
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="2:18">
+    <row r="60" spans="1:18">
       <c r="B60" t="s">
         <v>56</v>
       </c>
@@ -2322,7 +2336,10 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="2:18">
+    <row r="61" spans="1:18">
+      <c r="A61" t="s">
+        <v>219</v>
+      </c>
       <c r="B61" t="s">
         <v>81</v>
       </c>
@@ -2335,7 +2352,10 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="2:18">
+    <row r="62" spans="1:18">
+      <c r="A62" t="s">
+        <v>219</v>
+      </c>
       <c r="B62" t="s">
         <v>80</v>
       </c>
@@ -2352,7 +2372,10 @@
         <v>8.9978832245033585E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:18">
+    <row r="63" spans="1:18">
+      <c r="A63" t="s">
+        <v>219</v>
+      </c>
       <c r="B63" t="s">
         <v>79</v>
       </c>
@@ -2365,7 +2388,10 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="2:18">
+    <row r="64" spans="1:18">
+      <c r="A64" t="s">
+        <v>219</v>
+      </c>
       <c r="B64" t="s">
         <v>192</v>
       </c>
@@ -2421,6 +2447,9 @@
       </c>
     </row>
     <row r="67" spans="1:20">
+      <c r="A67" t="s">
+        <v>219</v>
+      </c>
       <c r="B67" t="s">
         <v>36</v>
       </c>
@@ -2438,6 +2467,9 @@
       </c>
     </row>
     <row r="68" spans="1:20">
+      <c r="A68" t="s">
+        <v>219</v>
+      </c>
       <c r="B68" t="s">
         <v>137</v>
       </c>
@@ -2451,6 +2483,9 @@
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:20">
+      <c r="A69" t="s">
+        <v>219</v>
+      </c>
       <c r="B69" t="s">
         <v>39</v>
       </c>
@@ -2467,6 +2502,9 @@
       </c>
     </row>
     <row r="70" spans="1:20" ht="31.35">
+      <c r="A70" t="s">
+        <v>219</v>
+      </c>
       <c r="B70" t="s">
         <v>133</v>
       </c>
@@ -2599,6 +2637,9 @@
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:20">
+      <c r="A80" t="s">
+        <v>219</v>
+      </c>
       <c r="B80" t="s">
         <v>194</v>
       </c>
@@ -2647,6 +2688,9 @@
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:17">
+      <c r="A84" t="s">
+        <v>220</v>
+      </c>
       <c r="B84" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Made the ion_dens function faster
</commit_message>
<xml_diff>
--- a/orfeas_competition/Mirror0D.xlsx
+++ b/orfeas_competition/Mirror0D.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/Python Scripts/orfeas_competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{C9E569C6-D225-2449-81CE-F63B9459901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9C307E8-E450-41C3-813B-78CFD08C0D8B}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{C9E569C6-D225-2449-81CE-F63B9459901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{945E32CD-6802-4970-AEE2-CC2303B2F078}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FD75F1BD-3419-8A42-869C-4E4296CA182A}"/>
   </bookViews>
@@ -1283,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6664DC-0609-414F-AD6B-0794283356C6}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="101" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="101" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.7"/>

</xml_diff>

<commit_message>
Added reduced model for Ti and Te. Can now calculate Q
</commit_message>
<xml_diff>
--- a/orfeas_competition/Mirror0D.xlsx
+++ b/orfeas_competition/Mirror0D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sanwalka_wisc_edu/Documents/WHAM/Python Scripts/orfeas_competition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/Things/Plasma-Projects/wham/orfeas_competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{C9E569C6-D225-2449-81CE-F63B9459901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{945E32CD-6802-4970-AEE2-CC2303B2F078}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E462C799-39D7-B34C-85D8-EFECEC061583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FD75F1BD-3419-8A42-869C-4E4296CA182A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35340" windowHeight="28300" xr2:uid="{FD75F1BD-3419-8A42-869C-4E4296CA182A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,6 +79,7 @@
     <definedName name="Zeff">Sheet1!$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -90,7 +91,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1283,11 +1283,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6664DC-0609-414F-AD6B-0794283356C6}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="101" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
@@ -1309,7 +1309,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18">
+    <row r="2" spans="1:8" ht="19">
       <c r="B2" s="22" t="s">
         <v>116</v>
       </c>
@@ -1673,10 +1673,9 @@
         <v>141</v>
       </c>
       <c r="D24" s="9">
-        <f>0.66*Einj</f>
-        <v>660</v>
-      </c>
-      <c r="E24" s="9"/>
+        <f>2/3*Einj</f>
+        <v>666.66666666666663</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -1709,7 +1708,7 @@
         <f>0.089*Einj*LOG10(Rmirror)^0.4</f>
         <v>77.121136715649044</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -1823,7 +1822,7 @@
       </c>
       <c r="D29" s="1">
         <f>D4^2*D9/0.04/( D24 + D26)</f>
-        <v>0.97677296734165731</v>
+        <v>0.96801802439601381</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
@@ -1859,7 +1858,7 @@
       </c>
       <c r="D30" s="1">
         <f>D29</f>
-        <v>0.97677296734165731</v>
+        <v>0.96801802439601381</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="9"/>
@@ -1892,7 +1891,7 @@
       </c>
       <c r="D31" s="1">
         <f>0.0031*SQRT(mu)*SQRT(Eion)/Bp</f>
-        <v>2.0987099211976234E-2</v>
+        <v>2.1092828340632922E-2</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
@@ -1918,7 +1917,7 @@
       </c>
       <c r="D33" s="1">
         <f>0.028*SQRT(mu/n_20)</f>
-        <v>4.4795173164494467E-2</v>
+        <v>4.4997285329063941E-2</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
@@ -1931,7 +1930,7 @@
       </c>
       <c r="D34" s="1">
         <f>97900*SQRT(Eion*1000/mu)</f>
-        <v>50301930.77805265</v>
+        <v>50555342.612494141</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
@@ -1944,7 +1943,7 @@
       </c>
       <c r="D35" s="1">
         <f>D34/D8</f>
-        <v>12575482.694513163</v>
+        <v>12638835.653123535</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>205</v>
@@ -1965,7 +1964,7 @@
       </c>
       <c r="D36" s="10">
         <f>D16/D31</f>
-        <v>26.636220124024852</v>
+        <v>26.502704395411264</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="7"/>
@@ -1978,7 +1977,7 @@
       </c>
       <c r="D37" s="10">
         <f>D16/D33</f>
-        <v>12.479402464237715</v>
+        <v>12.423349326228708</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="7"/>
@@ -2034,7 +2033,7 @@
       </c>
       <c r="D41" s="9">
         <f>2100*SQRT(D29/2)</f>
-        <v>1467.5777297943555</v>
+        <v>1460.9858807644962</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="1"/>
@@ -2056,7 +2055,7 @@
       </c>
       <c r="D42" s="7">
         <f>90*SQRT(D30)</f>
-        <v>88.948642684795502</v>
+        <v>88.549116300546515</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="1"/>
@@ -2073,7 +2072,7 @@
       </c>
       <c r="D43" s="7">
         <f>2*D16^2/D8/D31</f>
-        <v>7.4450498576209316</v>
+        <v>7.4077310769652582</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="1"/>
@@ -2091,7 +2090,7 @@
       </c>
       <c r="D44" s="1">
         <f>(D41/D39)^2</f>
-        <v>1063.5972311053602</v>
+        <v>1054.0640710089929</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
@@ -2273,7 +2272,7 @@
       </c>
       <c r="D56">
         <f>SQRT(90*D38/D42^2/D50)</f>
-        <v>0.10303868741864829</v>
+        <v>0.10350358956496004</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2329,7 +2328,7 @@
       </c>
       <c r="D60" s="1">
         <f>D30*D19</f>
-        <v>3.8338338968160057</v>
+        <v>3.7994707457543551</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -2345,7 +2344,7 @@
       </c>
       <c r="D61" s="1">
         <f xml:space="preserve"> 31 - 0.5 *LN(10^20) - 0.5 * LN(n_20) + LN(1000*Te)</f>
-        <v>19.239032254445604</v>
+        <v>19.243534024623031</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -2361,7 +2360,7 @@
       </c>
       <c r="D62" s="1">
         <f xml:space="preserve"> 24 - 0.5 *LN(10^14) - 0.5 * LN(n_20) +  LN(1000*Te)</f>
-        <v>19.146787533427741</v>
+        <v>19.151289303605168</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -2381,7 +2380,7 @@
       </c>
       <c r="D63" s="1">
         <f xml:space="preserve"> 23.5 - 0.5 *LN(10^14) - 0.5 * LN(n_20) + 1.5* LN(1000*Te) - (0.00001 + ( LN(1000*Te) - 2)^2 / 16)^0.5</f>
-        <v>21.96006853918508</v>
+        <v>21.964570309362507</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -2397,7 +2396,7 @@
       </c>
       <c r="D64" s="1">
         <f>0.00000000344*1000^1.5*Te^1.5/lambda_ei</f>
-        <v>3.8478900834711368E-3</v>
+        <v>3.8469855847426604E-3</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -2410,7 +2409,7 @@
       </c>
       <c r="D65" s="1" cm="1">
         <f t="array" ref="D65">0.0001*Te^1.5/n_20/lambda_ee</f>
-        <v>3.1574233051324357E-3</v>
+        <v>3.1853266688894035E-3</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -2431,7 +2430,7 @@
       </c>
       <c r="D66" s="1">
         <f>0.000125*Eion^1.5*mu^0.5/n_20/Zeff^4</f>
-        <v>2.617382402105203</v>
+        <v>2.681171375190345</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -2455,7 +2454,7 @@
       </c>
       <c r="D67" s="1">
         <f>0.1*Te^1.5*mu/n_20/1^2/lambda_ei</f>
-        <v>9.0533767174878559</v>
+        <v>9.1331098481106174</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -2475,14 +2474,14 @@
       </c>
       <c r="D68" s="1">
         <f>0.1*Te^1.5*4/n_20/2^2/lambda_ei</f>
-        <v>3.6213506869951426</v>
+        <v>3.6532439392442475</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" ht="17">
       <c r="A69" t="s">
         <v>219</v>
       </c>
@@ -2491,7 +2490,7 @@
       </c>
       <c r="D69" s="1">
         <f>1/( 1/tau_ii/0.4/LN(Rmirror/SQRT(1-beta) ) + 1/tau_s )</f>
-        <v>1.9758841800512887</v>
+        <v>2.01724649856259</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -2501,7 +2500,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="31.35">
+    <row r="70" spans="1:20" ht="51">
       <c r="A70" t="s">
         <v>219</v>
       </c>
@@ -2510,7 +2509,7 @@
       </c>
       <c r="D70" s="1">
         <f>0.00028*Einj^1.5 *LOG10( BM/Bp/SQRT(1-beta) ) / n_20</f>
-        <v>9.5041700330749386</v>
+        <v>9.5901275920131432</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
@@ -2539,7 +2538,7 @@
       </c>
       <c r="D72" s="1">
         <f>D60*100000000000000000000/D70</f>
-        <v>4.0338439689884459E+19</v>
+        <v>3.9618563041003053E+19</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -2559,7 +2558,7 @@
       </c>
       <c r="D74" s="1">
         <f>D72*1.6E-19</f>
-        <v>6.4541503503815134</v>
+        <v>6.3389700865604883</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -2609,7 +2608,7 @@
       </c>
       <c r="D77" s="17">
         <f ca="1">FORECAST(Eion,OFFSET($L$21:$L$30,MATCH(Eion,$K$21:$K$30,1)-1,0,2), OFFSET($K$21:$K$30,MATCH(Eion,$K$21:$K$30,1)-1,0,2))</f>
-        <v>3.38E+18</v>
+        <v>3.366666666666667E+18</v>
       </c>
       <c r="E77" s="17"/>
       <c r="F77" s="1"/>
@@ -2622,7 +2621,7 @@
       </c>
       <c r="D78" s="17">
         <f ca="1">FORECAST(0.66*Eion,OFFSET($M$24:$M$30,MATCH(Eion,$K$24:$K$30,1)-1,0,2), OFFSET($K$24:$K$30,MATCH(Eion,$K$24:$K$30,1)-1,0,2))</f>
-        <v>1.74848E+18</v>
+        <v>1.752E+18</v>
       </c>
       <c r="E78" s="17"/>
       <c r="F78" s="1"/>
@@ -2645,7 +2644,7 @@
       </c>
       <c r="D80" s="1">
         <f>D16^2*D64/D32^2</f>
-        <v>99094.110560435598</v>
+        <v>99070.817146367874</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -2680,14 +2679,14 @@
       </c>
       <c r="D83" s="1">
         <f>I_nbi*Einj*0.001/tau_s</f>
-        <v>0.71289978886158856</v>
+        <v>0.69406480289644634</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" ht="17">
       <c r="A84" t="s">
         <v>220</v>
       </c>
@@ -2696,7 +2695,7 @@
       </c>
       <c r="D84" s="1" cm="1">
         <f t="array" ref="D84">0.006*volume*n_20*Te*gamma_lorentz^2*Bp^2</f>
-        <v>73.503218157735802</v>
+        <v>72.844399268589498</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -2712,7 +2711,7 @@
       </c>
       <c r="D85" s="1">
         <f>5350*n_20^2*Zeff*SQRT(Te)*volume*0.000001</f>
-        <v>0.18825702679911668</v>
+        <v>0.1848974065802288</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -2725,7 +2724,7 @@
       </c>
       <c r="D86" s="1">
         <f>(I_nbi+I_cool)*7*Te*0.001</f>
-        <v>3.4842598808858884</v>
+        <v>3.4220800507742881</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -2745,14 +2744,14 @@
       </c>
       <c r="D88" s="1">
         <f>D75*1000*D74*0.000001</f>
-        <v>6.4541503503815125</v>
+        <v>6.3389700865604883</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:17" ht="16" thickBot="1">
+    <row r="89" spans="1:17" ht="18" thickBot="1">
       <c r="B89" t="s">
         <v>8</v>
       </c>
@@ -2774,13 +2773,13 @@
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="1:17" ht="16.350000000000001" thickTop="1" thickBot="1">
+    <row r="90" spans="1:17" ht="19" thickTop="1" thickBot="1">
       <c r="B90" t="s">
         <v>82</v>
       </c>
       <c r="D90" s="1">
         <f>I_nbi*(Einj - Te)*0.001</f>
-        <v>5.9563989388263865</v>
+        <v>5.8501015078784464</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -2791,13 +2790,13 @@
       </c>
       <c r="Q90" s="5"/>
     </row>
-    <row r="91" spans="1:17" s="5" customFormat="1" ht="32" thickTop="1" thickBot="1">
+    <row r="91" spans="1:17" s="5" customFormat="1" ht="36" thickTop="1" thickBot="1">
       <c r="B91" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D91" s="6">
         <f>MAX(0.05*Psynch +Pe_endloss -D83,0)</f>
-        <v>6.4465209999110895</v>
+        <v>6.3702352113073166</v>
       </c>
       <c r="E91" s="6"/>
       <c r="F91" s="6"/>
@@ -2806,6 +2805,7 @@
       <c r="I91" s="26" t="s">
         <v>142</v>
       </c>
+      <c r="J91"/>
       <c r="K91"/>
       <c r="L91"/>
       <c r="M91"/>
@@ -2814,13 +2814,13 @@
       <c r="P91"/>
       <c r="Q91"/>
     </row>
-    <row r="92" spans="1:17" ht="16" thickTop="1">
+    <row r="92" spans="1:17" ht="17" thickTop="1">
       <c r="B92" t="s">
         <v>10</v>
       </c>
       <c r="D92" s="1">
         <f>D91+D89+D88</f>
-        <v>12.900671350292601</v>
+        <v>12.709205297867804</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D94" s="1">
         <f>D70*D29*Eion</f>
-        <v>6127.0548011153342</v>
+        <v>6188.9442435508427</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>189</v>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="D95" s="3">
         <f ca="1">0.25*volume*sigma_v_dt*n_20^2</f>
-        <v>3.1643435883763589E+18</v>
+        <v>3.0956131055884467E+18</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="1"/>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="D96" s="1">
         <f ca="1" xml:space="preserve"> volume*sigma_v_dd*n_20^2</f>
-        <v>6.5476822217802322E+18</v>
+        <v>6.4437792011773757E+18</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="D97" s="1">
         <f ca="1">D95*17.6*1.6E-19</f>
-        <v>8.910791544867827</v>
+        <v>8.7172465053370658</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="D99" s="1">
         <f ca="1">D97/D92</f>
-        <v>0.69072308742023114</v>
+        <v>0.6859002039096449</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -2924,7 +2924,7 @@
       </c>
       <c r="D100" s="1">
         <f ca="1">D97/(4*3.14*D16^2*D17^2)*14/17.6</f>
-        <v>1.4924734722246755</v>
+        <v>1.4600565050309242</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D101" s="1">
         <f ca="1">D95/D72</f>
-        <v>7.8444868287006933E-2</v>
+        <v>7.8135421074829389E-2</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="D103" s="1">
         <f ca="1">I_nbi*D99*D68*E_nbi/D58/16/volume</f>
-        <v>7.3449009923791261E-2</v>
+        <v>7.2265434576169768E-2</v>
       </c>
       <c r="E103" s="1"/>
     </row>
@@ -2960,7 +2960,7 @@
       </c>
       <c r="D104" s="1">
         <f ca="1">1 + 2*D103</f>
-        <v>1.1468980198475824</v>
+        <v>1.1445308691523395</v>
       </c>
       <c r="E104" s="1"/>
     </row>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="D110" s="1">
         <f>D92/D107 - D106*D92*(1 - Te/Einj)</f>
-        <v>7.7143492801912767</v>
+        <v>7.5998563236932561</v>
       </c>
       <c r="E110" s="1"/>
     </row>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="D111" s="1">
         <f ca="1">0.8*D97*D107</f>
-        <v>4.9900432651259834</v>
+        <v>4.8816580429887564</v>
       </c>
       <c r="E111" s="1"/>
       <c r="I111" s="28"/>
@@ -3051,13 +3051,13 @@
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" ht="17">
       <c r="B114" t="s">
         <v>146</v>
       </c>
       <c r="D114" s="1">
         <f ca="1">D99/(1/D107 - D106*(1 - Te/Einj+0.2*D99))</f>
-        <v>1.458297595142672</v>
+        <v>1.4454659342086205</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="D116" s="1">
         <f ca="1">D114*0.8*D107</f>
-        <v>0.81664665327989638</v>
+        <v>0.80946092315682738</v>
       </c>
       <c r="E116" s="1"/>
     </row>
@@ -3326,14 +3326,14 @@
       </c>
       <c r="D143" s="1">
         <f>5*D92</f>
-        <v>64.503356751463002</v>
+        <v>63.54602648933902</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="31.7">
+    <row r="145" spans="1:10" ht="35">
       <c r="B145" s="23" t="s">
         <v>114</v>
       </c>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="J145" s="4"/>
     </row>
-    <row r="146" spans="1:10" ht="18">
+    <row r="146" spans="1:10" ht="19">
       <c r="B146" s="32"/>
       <c r="C146" s="33"/>
       <c r="D146" s="33"/>
@@ -3400,13 +3400,13 @@
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
     </row>
-    <row r="150" spans="1:10" ht="31.35">
+    <row r="150" spans="1:10" ht="34">
       <c r="B150" t="s">
         <v>97</v>
       </c>
       <c r="D150" s="1">
         <f>2*D92</f>
-        <v>25.801342700585202</v>
+        <v>25.418410595735608</v>
       </c>
       <c r="E150" s="1"/>
       <c r="I150" s="24" t="s">
@@ -3424,7 +3424,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" ht="17">
       <c r="A155" t="s">
         <v>15</v>
       </c>
@@ -3455,14 +3455,14 @@
       </c>
       <c r="D158" s="7">
         <f>D154*n_20</f>
-        <v>0.27349643085566405</v>
+        <v>0.27104504683088387</v>
       </c>
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
       <c r="H158" s="7"/>
     </row>
-    <row r="159" spans="1:10" ht="31.35">
+    <row r="159" spans="1:10" ht="34">
       <c r="B159" t="s">
         <v>27</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" ht="17">
       <c r="B160" t="s">
         <v>30</v>
       </c>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="D161" s="7">
         <f>0.04*D158*(Tic+D160)/D147^2</f>
-        <v>0.99845470462777375</v>
+        <v>0.98950542545534159</v>
       </c>
       <c r="E161" s="7"/>
       <c r="F161" s="7"/>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="D162" s="7">
         <f>0.000125*D159^1.5*SQRT(2.5)/D158</f>
-        <v>0.48942763474507683</v>
+        <v>0.49385411329219681</v>
       </c>
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
@@ -3524,7 +3524,7 @@
       </c>
       <c r="D163" s="10">
         <f>LN(2*D5/D147/SQRT(1-D161)+1)*LN(D30/D158)*(D30/D158)^(D26/D159)</f>
-        <v>32.138299644744158</v>
+        <v>27.789958502241976</v>
       </c>
       <c r="E163" s="10"/>
       <c r="F163" s="10"/>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="D168" s="10">
         <f>D163*D162</f>
-        <v>15.729371979855676</v>
+        <v>13.724185314551656</v>
       </c>
       <c r="E168" s="10"/>
       <c r="F168" s="10" t="s">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="D170" s="10">
         <f>D158*D159*D168</f>
-        <v>331.76950771843667</v>
+        <v>286.88079188135907</v>
       </c>
       <c r="E170" s="10"/>
       <c r="F170" s="10"/>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="D171" s="1">
         <f>1.5*0.016*3.14*D148^2*D158*(D160+D159)/D168</f>
-        <v>0.2915026501502424</v>
+        <v>0.33109843578323461</v>
       </c>
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="D173" s="1">
         <f ca="1">3.14*D148^2*0.25*D158^2*D172</f>
-        <v>7.2761338284388659E+17</v>
+        <v>7.1462845115714432E+17</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="D176" s="1">
         <f ca="1">D173*17.6*1.6E-19</f>
-        <v>2.0489592860883845</v>
+        <v>2.0123937184585183</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="D177" s="10">
         <f ca="1">D150/D176</f>
-        <v>12.592413561248394</v>
+        <v>12.630933182998584</v>
       </c>
       <c r="E177" s="10"/>
       <c r="F177" s="10"/>
@@ -3704,19 +3704,19 @@
       </c>
       <c r="D179" s="10">
         <f ca="1">D177*D176+D97*2</f>
-        <v>43.622925790320856</v>
+        <v>42.85290360640974</v>
       </c>
       <c r="E179" s="10"/>
       <c r="F179" s="10"/>
       <c r="G179" s="10"/>
       <c r="H179" s="10"/>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" ht="17">
       <c r="I182" s="24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="18">
+    <row r="183" spans="1:9" ht="19">
       <c r="B183" s="22" t="s">
         <v>115</v>
       </c>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="D185">
         <f ca="1">D184*D177</f>
-        <v>125.92413561248394</v>
+        <v>126.30933182998584</v>
       </c>
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="D186" s="10">
         <f ca="1">2*D97+ D176*D185</f>
-        <v>275.83501009558768</v>
+        <v>271.6185989680302</v>
       </c>
       <c r="E186" s="10"/>
       <c r="F186" s="10" t="s">
@@ -3773,13 +3773,13 @@
       <c r="G187" s="10"/>
       <c r="H187" s="10"/>
     </row>
-    <row r="188" spans="1:9" ht="31.35">
+    <row r="188" spans="1:9" ht="34">
       <c r="B188" t="s">
         <v>90</v>
       </c>
       <c r="D188" s="10">
         <f ca="1">3.14*D148^2*D185*D158*16/D168</f>
-        <v>158.65611258756743</v>
+        <v>180.75815085527978</v>
       </c>
       <c r="E188" s="10"/>
       <c r="F188" s="10" t="s">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="D190" s="1">
         <f ca="1">D185*D171</f>
-        <v>36.707219248917589</v>
+        <v>41.820822193733839</v>
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="7" t="s">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="D191">
         <f ca="1">0.2*D186</f>
-        <v>55.16700201911754</v>
+        <v>54.323719793606045</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="D192" s="1">
         <f>D92</f>
-        <v>12.900671350292601</v>
+        <v>12.709205297867804</v>
       </c>
       <c r="E192" s="1"/>
     </row>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="D193" s="1">
         <f ca="1">D190-D191-D192</f>
-        <v>-31.360454120492552</v>
+        <v>-25.21210289774001</v>
       </c>
       <c r="E193" s="1"/>
     </row>
@@ -3853,20 +3853,20 @@
       </c>
       <c r="D196" s="1">
         <f>2*D91</f>
-        <v>12.893041999822179</v>
+        <v>12.740470422614633</v>
       </c>
       <c r="E196" s="1"/>
       <c r="F196" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="2:9">
+    <row r="197" spans="2:9" ht="17">
       <c r="B197" s="18" t="s">
         <v>101</v>
       </c>
       <c r="D197" s="1">
         <f>2*D88</f>
-        <v>12.908300700763025</v>
+        <v>12.677940173120977</v>
       </c>
       <c r="E197" s="1"/>
       <c r="F197" s="7" t="s">
@@ -3876,7 +3876,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="198" spans="2:9" ht="16" thickBot="1">
+    <row r="198" spans="2:9" ht="17" thickBot="1">
       <c r="B198" s="18" t="s">
         <v>102</v>
       </c>
@@ -3889,13 +3889,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="199" spans="2:9" ht="16" thickTop="1">
+    <row r="199" spans="2:9" ht="17" thickTop="1">
       <c r="B199" s="21" t="s">
         <v>106</v>
       </c>
       <c r="D199" s="1">
         <f>SUM(D196:D198)</f>
-        <v>25.801342700585202</v>
+        <v>25.418410595735608</v>
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="7" t="s">
@@ -3914,7 +3914,7 @@
       </c>
       <c r="D202" s="1">
         <f ca="1">D186+2*D97</f>
-        <v>293.65659318532335</v>
+        <v>289.05309197870434</v>
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="7" t="s">
@@ -3927,14 +3927,14 @@
       </c>
       <c r="D204" s="1">
         <f ca="1">D106*(0.2*D202+D190+D90)</f>
-        <v>91.255443142327792</v>
+        <v>94.933387887617855</v>
       </c>
       <c r="E204" s="1"/>
       <c r="F204" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="205" spans="2:9">
+    <row r="205" spans="2:9" ht="17">
       <c r="I205" s="24" t="s">
         <v>135</v>
       </c>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="D206" s="1">
         <f ca="1">0.8*D202+ (1 - D106)*D204/D106</f>
-        <v>245.06476823073956</v>
+        <v>241.79062779269881</v>
       </c>
       <c r="E206" s="1"/>
       <c r="F206" s="7" t="s">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="D209" s="1">
         <f>D196/0.6</f>
-        <v>21.488403333036967</v>
+        <v>21.234117371024389</v>
       </c>
       <c r="E209" s="1"/>
       <c r="F209" s="7" t="s">
@@ -3976,14 +3976,14 @@
       </c>
       <c r="D210" s="1">
         <f>D197/0.6</f>
-        <v>21.51383450127171</v>
+        <v>21.129900288534962</v>
       </c>
       <c r="E210" s="1"/>
       <c r="F210" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="16" thickBot="1">
+    <row r="211" spans="1:8" ht="17" thickBot="1">
       <c r="B211" s="18" t="s">
         <v>111</v>
       </c>
@@ -3996,10 +3996,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="16" thickTop="1">
+    <row r="212" spans="1:8" ht="17" thickTop="1">
       <c r="D212" s="1">
         <f>SUM(D209:D211)</f>
-        <v>43.002237834308673</v>
+        <v>42.364017659559352</v>
       </c>
       <c r="E212" s="1"/>
       <c r="F212" s="7" t="s">
@@ -4012,7 +4012,7 @@
       </c>
       <c r="D214" s="1">
         <f ca="1">D204-D212</f>
-        <v>48.253205308019119</v>
+        <v>52.569370228058503</v>
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="7" t="s">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D216" s="1">
         <f ca="1">D206*0.5</f>
-        <v>122.53238411536978</v>
+        <v>120.89531389634941</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="7" t="s">
@@ -4043,7 +4043,7 @@
       </c>
       <c r="D218" s="1">
         <f ca="1">D216+D214</f>
-        <v>170.7855894233889</v>
+        <v>173.46468412440791</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="7" t="s">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="D222" s="1">
         <f ca="1">D176/2/3.14/D148</f>
-        <v>0.27167190319366818</v>
+        <v>0.26682366759581649</v>
       </c>
       <c r="E222" s="1"/>
       <c r="F222" s="1"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="D228" s="7">
         <f ca="1">D185*D227</f>
-        <v>155.59497855993152</v>
+        <v>156.07093653980615</v>
       </c>
       <c r="E228" s="7"/>
       <c r="F228" t="s">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="D230">
         <f ca="1">3.14*(D225^2 - D223^2)*D185</f>
-        <v>759.62747897106635</v>
+        <v>761.9511449639831</v>
       </c>
       <c r="F230" t="s">
         <v>122</v>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="D233" s="1">
         <f>10*2*D91</f>
-        <v>128.93041999822179</v>
+        <v>127.40470422614634</v>
       </c>
       <c r="E233" s="1"/>
     </row>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="D235" s="1">
         <f>5*2*D88</f>
-        <v>64.541503503815122</v>
+        <v>63.38970086560488</v>
       </c>
       <c r="E235" s="1"/>
     </row>

</xml_diff>

<commit_message>
update (sorry it isn't more descriptive)
</commit_message>
<xml_diff>
--- a/orfeas_competition/Mirror0D.xlsx
+++ b/orfeas_competition/Mirror0D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/Things/Plasma-Projects/wham/orfeas_competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E462C799-39D7-B34C-85D8-EFECEC061583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42383597-C896-E840-9D64-2B9396F565B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35340" windowHeight="28300" xr2:uid="{FD75F1BD-3419-8A42-869C-4E4296CA182A}"/>
+    <workbookView xWindow="-38700" yWindow="2680" windowWidth="37360" windowHeight="25700" xr2:uid="{FD75F1BD-3419-8A42-869C-4E4296CA182A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,8 +78,7 @@
     <definedName name="Wloss">Sheet1!#REF!</definedName>
     <definedName name="Zeff">Sheet1!$D$12</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,10 +86,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -98,14 +94,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -1283,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6664DC-0609-414F-AD6B-0794283356C6}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J159" sqref="J159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -3285,7 +3281,6 @@
       <c r="D139" s="1">
         <v>1E-4</v>
       </c>
-      <c r="E139" s="1"/>
       <c r="F139" t="s">
         <v>158</v>
       </c>

</xml_diff>